<commit_message>
testing backend.py and images for readme
</commit_message>
<xml_diff>
--- a/app/static/data/admin/KPIs.xlsx
+++ b/app/static/data/admin/KPIs.xlsx
@@ -58,6 +58,74 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -362,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H31"/>
+  <dimension ref="A1:H49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
@@ -1232,6 +1300,506 @@
         <v>44027.656118279</v>
       </c>
     </row>
+    <row r="32">
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>High School</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>District of Columbia</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>out-of-state</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Education</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>Less than 1 Year</t>
+        </is>
+      </c>
+      <c r="H32" s="3" t="n">
+        <v>44027.66921391546</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>High School</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Iowa</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>out-of-state</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>Education</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>Less than 1 Year</t>
+        </is>
+      </c>
+      <c r="H33" s="3" t="n">
+        <v>44027.66937459796</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>High School</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>District of Columbia</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>out-of-state</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>Education</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>Less than 1 Year</t>
+        </is>
+      </c>
+      <c r="H34" s="3" t="n">
+        <v>44027.66950079981</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>High School</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>District of Columbia</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>out-of-state</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>Agriculture &amp; Natural Resources</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>Less than 1 Year</t>
+        </is>
+      </c>
+      <c r="H35" s="3" t="n">
+        <v>44027.66965874392</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>High School</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>District of Columbia</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>in-state</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>Agriculture &amp; Natural Resources</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>Less than 1 Year</t>
+        </is>
+      </c>
+      <c r="H36" s="3" t="n">
+        <v>44027.66973322234</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>High School</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Iowa</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>in-state</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>Humanities &amp; Liberal Arts</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>Less than 1 Year</t>
+        </is>
+      </c>
+      <c r="H37" s="3" t="n">
+        <v>44027.66982667609</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>High School</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>New York</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>out-of-state</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>Engineering</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>Less than 1 Year</t>
+        </is>
+      </c>
+      <c r="H38" s="3" t="n">
+        <v>44027.66995940193</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>High School</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>New Jersey</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>in-state</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>Education</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>Less than 1 Year</t>
+        </is>
+      </c>
+      <c r="H39" s="3" t="n">
+        <v>44027.67013829082</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>College</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>District of Columbia</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>Agriculture &amp; Natural Resources</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>10000</t>
+        </is>
+      </c>
+      <c r="H40" s="3" t="n">
+        <v>44027.67032781119</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>College</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>District of Columbia</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>Engineering</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>100000</t>
+        </is>
+      </c>
+      <c r="H41" s="3" t="n">
+        <v>44027.67051353793</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>College</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>New Jersey</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>Education</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>25000</t>
+        </is>
+      </c>
+      <c r="H42" s="3" t="n">
+        <v>44027.6708477892</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>College</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>New York</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>Education</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>25000</t>
+        </is>
+      </c>
+      <c r="H43" s="3" t="n">
+        <v>44027.67152561496</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>College</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>New York</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>Engineering</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>25000</t>
+        </is>
+      </c>
+      <c r="H44" s="3" t="n">
+        <v>44027.67189825617</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>College</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Michigan</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>Engineering</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>100000</t>
+        </is>
+      </c>
+      <c r="H45" s="3" t="n">
+        <v>44027.67257344551</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>College</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Illinois</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>Engineering</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>100000</t>
+        </is>
+      </c>
+      <c r="H46" s="3" t="n">
+        <v>44027.67270165341</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>High School</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>District of Columbia</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>in-state</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>Agriculture &amp; Natural Resources</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>Less than 1 Year</t>
+        </is>
+      </c>
+      <c r="H47" s="3" t="n">
+        <v>44027.67284026599</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>High School</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>New Jersey</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>in-state</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>Education</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>Less than 1 Year</t>
+        </is>
+      </c>
+      <c r="H48" s="3" t="n">
+        <v>44027.67912193229</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>College</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Alabama</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>Agriculture &amp; Natural Resources</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>25000</t>
+        </is>
+      </c>
+      <c r="H49" s="3" t="n">
+        <v>44027.68164028682</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
logging of user activity
</commit_message>
<xml_diff>
--- a/app/static/data/admin/KPIs.xlsx
+++ b/app/static/data/admin/KPIs.xlsx
@@ -1,12 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="15660" yWindow="810" windowWidth="9075" windowHeight="15480" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="15480" windowWidth="9075" xWindow="15660" yWindow="810"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="YTD_Status" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="YTD_Status" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -16,9 +16,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
-    <numFmt numFmtId="165" formatCode="yyyy/mm/dd\ h:mm:ss;@"/>
-    <numFmt numFmtId="166" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt formatCode="yyyy\-mm\-dd\ h:mm:ss" numFmtId="164"/>
+    <numFmt formatCode="yyyy/mm/dd\ h:mm:ss;@" numFmtId="165"/>
+    <numFmt formatCode="yyyy-mm-dd h:mm:ss" numFmtId="166"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -54,22 +54,22 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="44"/>
   </cellStyleXfs>
   <cellXfs count="6">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="166" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Currency" xfId="1" builtinId="4"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle builtinId="4" name="Currency" xfId="1"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -442,7 +442,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I575"/>
+  <dimension ref="A1:I577"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A435" workbookViewId="0">
       <selection activeCell="B450" sqref="B450"/>
@@ -450,15 +450,15 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="11.25" defaultRowHeight="15.75"/>
   <cols>
-    <col width="13.75" customWidth="1" min="1" max="1"/>
-    <col width="19.5" customWidth="1" min="2" max="2"/>
-    <col width="21.25" customWidth="1" min="3" max="3"/>
-    <col width="16.25" customWidth="1" min="4" max="4"/>
-    <col width="40.75" customWidth="1" min="5" max="5"/>
-    <col width="28.5" customWidth="1" min="6" max="6"/>
-    <col width="19.5" customWidth="1" min="7" max="7"/>
-    <col width="24.25" customWidth="1" min="8" max="8"/>
-    <col width="17.875" bestFit="1" customWidth="1" min="9" max="9"/>
+    <col customWidth="1" max="1" min="1" width="13.75"/>
+    <col customWidth="1" max="2" min="2" width="19.5"/>
+    <col customWidth="1" max="3" min="3" width="21.25"/>
+    <col customWidth="1" max="4" min="4" width="16.25"/>
+    <col customWidth="1" max="5" min="5" width="40.75"/>
+    <col customWidth="1" max="6" min="6" width="28.5"/>
+    <col customWidth="1" max="7" min="7" width="19.5"/>
+    <col customWidth="1" max="8" min="8" width="24.25"/>
+    <col bestFit="1" customWidth="1" max="9" min="9" width="17.875"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -16077,8 +16077,58 @@
         <v>44028.50768928446</v>
       </c>
     </row>
+    <row r="576">
+      <c r="B576" t="inlineStr">
+        <is>
+          <t>College</t>
+        </is>
+      </c>
+      <c r="C576" t="inlineStr">
+        <is>
+          <t>Illinois</t>
+        </is>
+      </c>
+      <c r="E576" t="inlineStr">
+        <is>
+          <t>Engineering</t>
+        </is>
+      </c>
+      <c r="G576" t="inlineStr">
+        <is>
+          <t>200000</t>
+        </is>
+      </c>
+      <c r="H576" s="5" t="n">
+        <v>44032.67448542513</v>
+      </c>
+    </row>
+    <row r="577">
+      <c r="B577" t="inlineStr">
+        <is>
+          <t>College</t>
+        </is>
+      </c>
+      <c r="C577" t="inlineStr">
+        <is>
+          <t>Illinois</t>
+        </is>
+      </c>
+      <c r="E577" t="inlineStr">
+        <is>
+          <t>Engineering</t>
+        </is>
+      </c>
+      <c r="G577" t="inlineStr">
+        <is>
+          <t>200000</t>
+        </is>
+      </c>
+      <c r="H577" s="5" t="n">
+        <v>44032.67578379867</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="300" orientation="portrait" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>